<commit_message>
Add translator files and update queries
</commit_message>
<xml_diff>
--- a/my_querys.xlsx
+++ b/my_querys.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="405">
   <si>
     <t xml:space="preserve">Zeitstempel</t>
   </si>
@@ -1209,6 +1209,24 @@
   </si>
   <si>
     <t xml:space="preserve">Wut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.02.2025_12.26.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gepflügter Boden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plowed soil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.02.2025_12.32.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erlöscht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expired</t>
   </si>
 </sst>
 </file>
@@ -4186,6 +4204,34 @@
         <v>398</v>
       </c>
     </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>399</v>
+      </c>
+      <c r="B190" t="s">
+        <v>186</v>
+      </c>
+      <c r="C190" t="s">
+        <v>400</v>
+      </c>
+      <c r="D190" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>402</v>
+      </c>
+      <c r="B191" t="s">
+        <v>186</v>
+      </c>
+      <c r="C191" t="s">
+        <v>403</v>
+      </c>
+      <c r="D191" t="s">
+        <v>404</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>